<commit_message>
added filters for the itemsets
</commit_message>
<xml_diff>
--- a/ConsoleApp1/bin/Debug/net8.0/Database1.xlsx
+++ b/ConsoleApp1/bin/Debug/net8.0/Database1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\otvyagis\Documents\GitHub\APRIORI\ConsoleApp1\bin\Debug\net8.0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\notso\OneDrive\Desktop\GitHub\APRIORI\ConsoleApp1\bin\Debug\net8.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89C5B174-1040-407E-9571-5DA850D34BD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E33B4D8-C44C-47C7-9B02-9BCE2B4B27FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -437,8 +437,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1299,7 +1299,7 @@
         <v>8</v>
       </c>
       <c r="C43" s="2">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="D43" s="2">
         <v>35000</v>
@@ -1339,7 +1339,7 @@
         <v>8</v>
       </c>
       <c r="C45" s="2">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="D45" s="2">
         <v>70090</v>

</xml_diff>